<commit_message>
benchmarkd result adds orleans
</commit_message>
<xml_diff>
--- a/docs/graph.xlsx
+++ b/docs/graph.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S04451\Documents\GitHub\MemoryPack\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\source\repos\MemoryPack\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7FBCB0C-6AD5-462D-AF77-B46E1F6CF57E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181EC602-5538-4E81-9603-DDCADB520B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12420" yWindow="2640" windowWidth="30690" windowHeight="24060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18195" yWindow="2625" windowWidth="57600" windowHeight="23535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>Method</t>
   </si>
@@ -59,6 +59,10 @@
   </si>
   <si>
     <t>Vector3[]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Orleans</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -113,7 +117,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -124,6 +128,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -221,7 +228,7 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
@@ -230,77 +237,6 @@
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>Deserialize(ns)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$M$17:$M$20</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>MemoryPack</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>MessagePack</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>protobuf-net</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>JsonSerializer</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$O$17:$O$20</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>25625</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>73863</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100461</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>440252</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-4B3E-4D6F-A9EF-9B6785EEBB78}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$N$16</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Serialize(ns)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -317,9 +253,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$M$17:$M$20</c:f>
+              <c:f>Sheet1!$M$17:$M$21</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>MemoryPack</c:v>
                 </c:pt>
@@ -327,9 +263,12 @@
                   <c:v>MessagePack</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Orleans</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>protobuf-net</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>JsonSerializer</c:v>
                 </c:pt>
               </c:strCache>
@@ -337,21 +276,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$17:$N$20</c:f>
+              <c:f>Sheet1!$O$17:$O$21</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>15073</c:v>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0" formatCode="#,##0">
+                  <c:v>24540</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43334</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>111277</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>271698</c:v>
+                  <c:v>39420</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="#,##0">
+                  <c:v>46210</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="#,##0">
+                  <c:v>51640</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="#,##0">
+                  <c:v>308900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -359,6 +301,83 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-4B3E-4D6F-A9EF-9B6785EEBB78}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Serialize(ns)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$M$17:$M$21</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>MemoryPack</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MessagePack</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Orleans</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>protobuf-net</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>JsonSerializer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$17:$N$21</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>13176</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22961</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58530</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>73028</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>189099</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4B3E-4D6F-A9EF-9B6785EEBB78}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -647,7 +666,7 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="2"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
@@ -656,77 +675,6 @@
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>Deserialize(ns)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$M$45:$M$48</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>MemoryPack</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>MessagePack</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>protobuf-net</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>JsonSerializer</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$O$45:$O$48</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>623</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>44032</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>60096</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>126605</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8BAB-4E3C-8EE7-FC49599CDDF8}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$N$44</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Serialize(ns)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -743,9 +691,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$M$45:$M$48</c:f>
+              <c:f>Sheet1!$M$45:$M$49</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>MemoryPack</c:v>
                 </c:pt>
@@ -753,9 +701,12 @@
                   <c:v>MessagePack</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Orleans</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>protobuf-net</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>JsonSerializer</c:v>
                 </c:pt>
               </c:strCache>
@@ -763,21 +714,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$45:$N$48</c:f>
+              <c:f>Sheet1!$O$45:$O$49</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>236</c:v>
+                  <c:v>316</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14280</c:v>
+                  <c:v>26335</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>81271</c:v>
+                  <c:v>41054</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>78201</c:v>
+                  <c:v>39526</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>77380</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -785,6 +739,83 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8BAB-4E3C-8EE7-FC49599CDDF8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$44</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Serialize(ns)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$M$45:$M$49</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>MemoryPack</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MessagePack</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Orleans</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>protobuf-net</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>JsonSerializer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$45:$N$49</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>231</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9887</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>53769</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49560</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8BAB-4E3C-8EE7-FC49599CDDF8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2128,7 +2159,7 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>228600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
@@ -2149,8 +2180,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4038600" y="7496175"/>
-          <a:ext cx="1828800" cy="581026"/>
+          <a:off x="4038600" y="7610475"/>
+          <a:ext cx="1828800" cy="466726"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2231,14 +2262,14 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>704850</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>228601</xdr:rowOff>
+      <xdr:rowOff>228600</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2253,8 +2284,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9344025" y="7505700"/>
-          <a:ext cx="1828800" cy="581026"/>
+          <a:off x="9344025" y="7667624"/>
+          <a:ext cx="1828800" cy="419101"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2296,15 +2327,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>933450</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1181100</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2319,8 +2350,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="10734675" y="7381875"/>
-          <a:ext cx="276225" cy="361950"/>
+          <a:off x="11401425" y="6076950"/>
+          <a:ext cx="2133600" cy="1714500"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2352,13 +2383,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>1152525</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>819150</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -2375,8 +2406,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="5372100" y="7391400"/>
-          <a:ext cx="247650" cy="266700"/>
+          <a:off x="5953125" y="6038850"/>
+          <a:ext cx="1619250" cy="1619250"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2408,11 +2439,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1009650</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>1457325</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1122359" cy="345544"/>
+    <xdr:ext cx="1242135" cy="345544"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="10" name="テキスト ボックス 9">
@@ -2426,70 +2457,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5810250" y="7486650"/>
-          <a:ext cx="1122359" cy="345544"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400">
-              <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>x3 faster!</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400">
-            <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1242135" cy="345544"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="テキスト ボックス 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06D12DBA-8790-4263-B812-C1127054DE50}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11134725" y="7496175"/>
+          <a:off x="6257925" y="7181850"/>
           <a:ext cx="1242135" cy="345544"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2521,7 +2489,70 @@
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400">
               <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>x50 faster!</a:t>
+            <a:t>x10 faster!</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400">
+            <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1503244</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1993973" cy="345544"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="テキスト ボックス 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06D12DBA-8790-4263-B812-C1127054DE50}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11971219" y="7191375"/>
+          <a:ext cx="1993973" cy="345544"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400">
+              <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>x200 faster!</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400">
             <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
@@ -2831,10 +2862,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="J15:AW48"/>
+  <dimension ref="J15:AW49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q48" sqref="Q48"/>
+      <selection activeCell="U46" sqref="U46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -2874,10 +2905,10 @@
         <v>5</v>
       </c>
       <c r="N17" s="3">
-        <v>15073</v>
+        <v>13176</v>
       </c>
       <c r="O17" s="3">
-        <v>25625</v>
+        <v>24540</v>
       </c>
       <c r="Q17"/>
     </row>
@@ -2886,42 +2917,48 @@
         <v>1</v>
       </c>
       <c r="N18" s="3">
-        <v>43334</v>
-      </c>
-      <c r="O18" s="3">
-        <v>73863</v>
+        <v>22961</v>
+      </c>
+      <c r="O18" s="1">
+        <v>39420</v>
       </c>
       <c r="Q18"/>
     </row>
     <row r="19" spans="13:49" x14ac:dyDescent="0.4">
       <c r="M19" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="N19" s="3">
-        <v>111277</v>
+        <v>58530</v>
       </c>
       <c r="O19" s="3">
-        <v>100461</v>
-      </c>
+        <v>46210</v>
+      </c>
+      <c r="P19"/>
       <c r="Q19"/>
     </row>
     <row r="20" spans="13:49" x14ac:dyDescent="0.4">
       <c r="M20" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="N20" s="3">
-        <v>271698</v>
+        <v>73028</v>
       </c>
       <c r="O20" s="3">
-        <v>440252</v>
+        <v>51640</v>
       </c>
       <c r="Q20"/>
     </row>
     <row r="21" spans="13:49" x14ac:dyDescent="0.4">
-      <c r="M21"/>
-      <c r="N21"/>
-      <c r="O21"/>
-      <c r="P21"/>
+      <c r="M21" t="s">
+        <v>6</v>
+      </c>
+      <c r="N21" s="3">
+        <v>189099</v>
+      </c>
+      <c r="O21" s="3">
+        <v>308900</v>
+      </c>
       <c r="Q21"/>
     </row>
     <row r="22" spans="13:49" x14ac:dyDescent="0.4">
@@ -3054,12 +3091,12 @@
       <c r="AS27"/>
       <c r="AT27"/>
     </row>
-    <row r="43" spans="13:15" x14ac:dyDescent="0.4">
+    <row r="43" spans="13:20" x14ac:dyDescent="0.4">
       <c r="M43" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="13:15" x14ac:dyDescent="0.4">
+    <row r="44" spans="13:20" x14ac:dyDescent="0.4">
       <c r="M44" t="s">
         <v>0</v>
       </c>
@@ -3070,48 +3107,67 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="13:15" x14ac:dyDescent="0.4">
+    <row r="45" spans="13:20" x14ac:dyDescent="0.4">
       <c r="M45" t="s">
         <v>5</v>
       </c>
       <c r="N45" s="3">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="O45" s="3">
-        <v>623</v>
-      </c>
+        <v>316</v>
+      </c>
+      <c r="S45" s="3"/>
+      <c r="T45" s="3"/>
     </row>
-    <row r="46" spans="13:15" x14ac:dyDescent="0.4">
+    <row r="46" spans="13:20" x14ac:dyDescent="0.4">
       <c r="M46" t="s">
         <v>1</v>
       </c>
       <c r="N46" s="3">
-        <v>14280</v>
+        <v>9887</v>
       </c>
       <c r="O46" s="3">
-        <v>44032</v>
-      </c>
+        <v>26335</v>
+      </c>
+      <c r="S46" s="3"/>
+      <c r="T46" s="3"/>
     </row>
-    <row r="47" spans="13:15" x14ac:dyDescent="0.4">
+    <row r="47" spans="13:20" x14ac:dyDescent="0.4">
       <c r="M47" t="s">
+        <v>9</v>
+      </c>
+      <c r="N47" s="4">
+        <v>42997</v>
+      </c>
+      <c r="O47" s="4">
+        <v>41054</v>
+      </c>
+      <c r="S47" s="3"/>
+      <c r="T47" s="3"/>
+    </row>
+    <row r="48" spans="13:20" x14ac:dyDescent="0.4">
+      <c r="M48" t="s">
         <v>4</v>
       </c>
-      <c r="N47" s="3">
-        <v>81271</v>
-      </c>
-      <c r="O47" s="3">
-        <v>60096</v>
-      </c>
+      <c r="N48" s="3">
+        <v>53769</v>
+      </c>
+      <c r="O48" s="3">
+        <v>39526</v>
+      </c>
+      <c r="S48" s="3"/>
+      <c r="T48" s="3"/>
     </row>
-    <row r="48" spans="13:15" x14ac:dyDescent="0.4">
-      <c r="M48" t="s">
+    <row r="49" spans="13:15" x14ac:dyDescent="0.4">
+      <c r="M49" t="s">
         <v>6</v>
       </c>
-      <c r="N48" s="3">
-        <v>78201</v>
-      </c>
-      <c r="O48" s="3">
-        <v>126605</v>
+      <c r="N49" s="3">
+        <v>49560</v>
+      </c>
+      <c r="O49" s="3">
+        <v>77380</v>
       </c>
     </row>
   </sheetData>

</xml_diff>